<commit_message>
Carpeta informes_vendor actualizada subida
</commit_message>
<xml_diff>
--- a/users/informes_vendor/miquelrius/tendencias de rendimiento/Tendencias de rendimiento de ventas_ES (1).xlsx
+++ b/users/informes_vendor/miquelrius/tendencias de rendimiento/Tendencias de rendimiento de ventas_ES (1).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd74f11e194d3d0b/Escritorio/pruebaVisualizacion/informes_vendor/miquelrius/tendencias de rendimiento/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mg_4_\OneDrive\Escritorio\pruebaVisualizacion\informes_vendor\miquelrius\tendencias de rendimiento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2EBCC3398C1E2C4FD647F3DD6FDF944DF62A8FB2" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{02317A6A-4672-4E1D-A04D-EBB7C9FC3E7A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2221E654-653A-4C24-AFFC-2BE213F4F254}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,6 +46,24 @@
     <t>Cambios en Conversión - Periodo anterior</t>
   </si>
   <si>
+    <t>02-jun-2020</t>
+  </si>
+  <si>
+    <t>01-jun-2020</t>
+  </si>
+  <si>
+    <t>31-may-2020</t>
+  </si>
+  <si>
+    <t>30-may-2020</t>
+  </si>
+  <si>
+    <t>29-may-2020</t>
+  </si>
+  <si>
+    <t>28-may-2020</t>
+  </si>
+  <si>
     <t>27-may-2020</t>
   </si>
   <si>
@@ -209,24 +227,6 @@
   </si>
   <si>
     <t>03-abr-2020</t>
-  </si>
-  <si>
-    <t>02-abr-2020</t>
-  </si>
-  <si>
-    <t>01-abr-2020</t>
-  </si>
-  <si>
-    <t>31-mar-2020</t>
-  </si>
-  <si>
-    <t>30-mar-2020</t>
-  </si>
-  <si>
-    <t>29-mar-2020</t>
-  </si>
-  <si>
-    <t>28-mar-2020</t>
   </si>
 </sst>
 </file>
@@ -286,9 +286,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -646,28 +646,28 @@
         <v>8</v>
       </c>
       <c r="B2" s="3">
-        <v>2822.9399999999978</v>
+        <v>2649.19</v>
       </c>
       <c r="C2" s="4">
-        <v>-0.10719571900261959</v>
+        <v>0.95150680289647926</v>
       </c>
       <c r="D2" s="5">
-        <v>528</v>
+        <v>451</v>
       </c>
       <c r="E2" s="4">
-        <v>-4.174228675136115E-2</v>
+        <v>0.85596707818930051</v>
       </c>
       <c r="F2" s="3">
-        <v>5.3464772727272685</v>
+        <v>5.8740354767184035</v>
       </c>
       <c r="G2" s="4">
-        <v>-6.8304623428870004E-2</v>
-      </c>
-      <c r="H2" s="4">
-        <v>-4.3519796199978922E-3</v>
-      </c>
-      <c r="I2" s="6">
-        <v>4.1266263435011608E-2</v>
+        <v>5.1477057879921295E-2</v>
+      </c>
+      <c r="H2" s="6">
+        <v>-2.8275318238143554E-2</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0.10363555302270244</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -675,28 +675,28 @@
         <v>9</v>
       </c>
       <c r="B3" s="3">
-        <v>3161.8800000000006</v>
-      </c>
-      <c r="C3" s="4">
-        <v>-1.8969786101233788E-2</v>
+        <v>1357.5100000000002</v>
+      </c>
+      <c r="C3" s="6">
+        <v>-0.19620219436664765</v>
       </c>
       <c r="D3" s="5">
-        <v>551</v>
+        <v>243</v>
       </c>
       <c r="E3" s="6">
-        <v>3.9622641509434064E-2</v>
+        <v>-0.20327868852459019</v>
       </c>
       <c r="F3" s="3">
-        <v>5.7384392014519063</v>
+        <v>5.5864609053497949</v>
       </c>
       <c r="G3" s="4">
-        <v>-5.6359322384126893E-2</v>
+        <v>8.8820194163476973E-3</v>
       </c>
       <c r="H3" s="4">
-        <v>-5.1067687348912205E-2</v>
-      </c>
-      <c r="I3" s="6">
-        <v>6.6879777111271466E-2</v>
+        <v>3.1010452961672375E-2</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0.24662682283500126</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -704,28 +704,28 @@
         <v>10</v>
       </c>
       <c r="B4" s="3">
-        <v>3223.0199999999991</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0.9977933291596679</v>
+        <v>1688.8700000000003</v>
+      </c>
+      <c r="C4" s="4">
+        <v>8.9614637702665423E-2</v>
       </c>
       <c r="D4" s="5">
-        <v>530</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0.66666666666666674</v>
+        <v>305</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.15530303030303028</v>
       </c>
       <c r="F4" s="3">
-        <v>6.0811698113207528</v>
+        <v>5.5372786885245917</v>
       </c>
       <c r="G4" s="6">
-        <v>0.19867599749580056</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0.32003722909187604</v>
+        <v>-5.6858149660643613E-2</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.41798418972332008</v>
       </c>
       <c r="I4" s="6">
-        <v>4.5378782025100595E-3</v>
+        <v>-0.10366252626539352</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -733,28 +733,28 @@
         <v>11</v>
       </c>
       <c r="B5" s="3">
-        <v>1613.2899999999993</v>
-      </c>
-      <c r="C5" s="4">
-        <v>-6.0489412751287282E-2</v>
+        <v>1549.97</v>
+      </c>
+      <c r="C5" s="6">
+        <v>-0.25369907601342401</v>
       </c>
       <c r="D5" s="5">
-        <v>318</v>
-      </c>
-      <c r="E5" s="4">
-        <v>-9.3457943925233655E-3</v>
+        <v>264</v>
+      </c>
+      <c r="E5" s="6">
+        <v>-0.32133676092544983</v>
       </c>
       <c r="F5" s="3">
-        <v>5.0732389937106896</v>
+        <v>5.8710984848484848</v>
       </c>
       <c r="G5" s="4">
-        <v>-5.1626105324412475E-2</v>
-      </c>
-      <c r="H5" s="4">
-        <v>-5.526943851274968E-2</v>
+        <v>9.9663103904462216E-2</v>
+      </c>
+      <c r="H5" s="6">
+        <v>-0.1214006656055564</v>
       </c>
       <c r="I5" s="6">
-        <v>4.7028572931653967E-2</v>
+        <v>-0.12806458944902877</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -762,28 +762,28 @@
         <v>12</v>
       </c>
       <c r="B6" s="3">
-        <v>1717.1599999999996</v>
-      </c>
-      <c r="C6" s="4">
-        <v>-0.32647185722690691</v>
+        <v>2076.87</v>
+      </c>
+      <c r="C6" s="6">
+        <v>-0.21725611686490864</v>
       </c>
       <c r="D6" s="5">
-        <v>321</v>
-      </c>
-      <c r="E6" s="4">
-        <v>-0.31702127659574464</v>
+        <v>389</v>
+      </c>
+      <c r="E6" s="6">
+        <v>-0.1506550218340611</v>
       </c>
       <c r="F6" s="3">
-        <v>5.3494080996884721</v>
-      </c>
-      <c r="G6" s="4">
-        <v>-1.3837298743446413E-2</v>
-      </c>
-      <c r="H6" s="4">
-        <v>-0.15263437998935603</v>
+        <v>5.3389974293059126</v>
+      </c>
+      <c r="G6" s="6">
+        <v>-7.841465687436544E-2</v>
+      </c>
+      <c r="H6" s="6">
+        <v>-0.20535816948372998</v>
       </c>
       <c r="I6" s="4">
-        <v>-0.10027421904927014</v>
+        <v>3.2092514383804671E-2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -791,28 +791,28 @@
         <v>13</v>
       </c>
       <c r="B7" s="3">
-        <v>2549.4999999999986</v>
-      </c>
-      <c r="C7" s="4">
-        <v>-0.268939611171647</v>
+        <v>2653.3199999999993</v>
+      </c>
+      <c r="C7" s="6">
+        <v>-6.0086293013666407E-2</v>
       </c>
       <c r="D7" s="5">
-        <v>470</v>
-      </c>
-      <c r="E7" s="4">
-        <v>-0.28024502297090348</v>
+        <v>458</v>
+      </c>
+      <c r="E7" s="6">
+        <v>-0.13257575757575757</v>
       </c>
       <c r="F7" s="3">
-        <v>5.4244680851063798</v>
-      </c>
-      <c r="G7" s="6">
-        <v>1.5707306180669178E-2</v>
-      </c>
-      <c r="H7" s="4">
-        <v>-0.13894235175510949</v>
+        <v>5.7932751091703043</v>
+      </c>
+      <c r="G7" s="4">
+        <v>8.356864036852428E-2</v>
+      </c>
+      <c r="H7" s="6">
+        <v>-7.2814498933901906E-2</v>
       </c>
       <c r="I7" s="6">
-        <v>2.1998935604044645E-2</v>
+        <v>-0.11466891923090505</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -820,28 +820,28 @@
         <v>14</v>
       </c>
       <c r="B8" s="3">
-        <v>3487.4000000000005</v>
+        <v>2822.9399999999987</v>
       </c>
       <c r="C8" s="6">
-        <v>4.0465187050424234E-2</v>
+        <v>-0.10719571900261894</v>
       </c>
       <c r="D8" s="5">
-        <v>653</v>
+        <v>528</v>
       </c>
       <c r="E8" s="6">
-        <v>1.5337423312884457E-3</v>
+        <v>-4.174228675136115E-2</v>
       </c>
       <c r="F8" s="3">
-        <v>5.3405819295558965</v>
+        <v>5.3464772727272702</v>
       </c>
       <c r="G8" s="6">
-        <v>3.8871825355094369E-2</v>
-      </c>
-      <c r="H8" s="4">
-        <v>-3.5616438356164126E-3</v>
+        <v>-6.8304623428869338E-2</v>
+      </c>
+      <c r="H8" s="6">
+        <v>-4.3519796199978922E-3</v>
       </c>
       <c r="I8" s="4">
-        <v>-8.1587510871121705E-2</v>
+        <v>4.1266263435011608E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -849,28 +849,28 @@
         <v>15</v>
       </c>
       <c r="B9" s="3">
-        <v>3351.77</v>
-      </c>
-      <c r="C9" s="4">
-        <v>-3.9973305301990614E-2</v>
+        <v>3161.8799999999992</v>
+      </c>
+      <c r="C9" s="6">
+        <v>-1.8969786101234898E-2</v>
       </c>
       <c r="D9" s="5">
-        <v>652</v>
+        <v>551</v>
       </c>
       <c r="E9" s="4">
-        <v>-4.6783625730994149E-2</v>
+        <v>3.9622641509434064E-2</v>
       </c>
       <c r="F9" s="3">
-        <v>5.1407515337423311</v>
+        <v>5.7384392014519046</v>
       </c>
       <c r="G9" s="6">
-        <v>7.144569284414537E-3</v>
-      </c>
-      <c r="H9" s="4">
-        <v>-5.9924450549450503E-2</v>
-      </c>
-      <c r="I9" s="6">
-        <v>0.2486529680365297</v>
+        <v>-5.6359322384127886E-2</v>
+      </c>
+      <c r="H9" s="6">
+        <v>-5.1067687348912205E-2</v>
+      </c>
+      <c r="I9" s="4">
+        <v>6.6879777111271466E-2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -878,28 +878,28 @@
         <v>16</v>
       </c>
       <c r="B10" s="3">
-        <v>3491.329999999999</v>
+        <v>3223.0200000000013</v>
       </c>
       <c r="C10" s="4">
-        <v>-7.9894794820911663E-2</v>
+        <v>0.99779332915966823</v>
       </c>
       <c r="D10" s="5">
-        <v>684</v>
+        <v>530</v>
       </c>
       <c r="E10" s="4">
-        <v>-7.1913161465400277E-2</v>
+        <v>0.66666666666666674</v>
       </c>
       <c r="F10" s="3">
-        <v>5.1042836257309929</v>
+        <v>6.0811698113207573</v>
       </c>
       <c r="G10" s="4">
-        <v>-8.6000932500174265E-3</v>
+        <v>0.198675997495801</v>
       </c>
       <c r="H10" s="4">
-        <v>-4.8366013071895475E-2</v>
+        <v>0.32003722909187604</v>
       </c>
       <c r="I10" s="4">
-        <v>-0.10329670329670326</v>
+        <v>4.5378782025100595E-3</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -907,28 +907,28 @@
         <v>17</v>
       </c>
       <c r="B11" s="3">
-        <v>3794.4900000000002</v>
+        <v>1613.2900000000002</v>
       </c>
       <c r="C11" s="6">
-        <v>0.61785723422217353</v>
+        <v>-6.0489412751286942E-2</v>
       </c>
       <c r="D11" s="5">
-        <v>737</v>
+        <v>318</v>
       </c>
       <c r="E11" s="6">
-        <v>0.59869848156182215</v>
+        <v>-9.3457943925233655E-3</v>
       </c>
       <c r="F11" s="3">
-        <v>5.1485617367706924</v>
+        <v>5.0732389937106923</v>
       </c>
       <c r="G11" s="6">
-        <v>1.1983968760409747E-2</v>
+        <v>-5.162610532441237E-2</v>
       </c>
       <c r="H11" s="6">
-        <v>4.2944785276073594E-2</v>
-      </c>
-      <c r="I11" s="6">
-        <v>0.10633484162895934</v>
+        <v>-5.526943851274968E-2</v>
+      </c>
+      <c r="I11" s="4">
+        <v>4.7028572931653967E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -936,28 +936,28 @@
         <v>18</v>
       </c>
       <c r="B12" s="3">
-        <v>2345.3799999999992</v>
+        <v>1717.16</v>
       </c>
       <c r="C12" s="6">
-        <v>7.4905817758507798E-2</v>
+        <v>-0.3264718572269073</v>
       </c>
       <c r="D12" s="5">
-        <v>461</v>
-      </c>
-      <c r="E12" s="7">
-        <v>0</v>
+        <v>321</v>
+      </c>
+      <c r="E12" s="6">
+        <v>-0.31702127659574464</v>
       </c>
       <c r="F12" s="3">
-        <v>5.0875921908893691</v>
+        <v>5.3494080996884739</v>
       </c>
       <c r="G12" s="6">
-        <v>7.4905817758507798E-2</v>
-      </c>
-      <c r="H12" s="4">
-        <v>-7.5541551792044137E-2</v>
+        <v>-1.3837298743446858E-2</v>
+      </c>
+      <c r="H12" s="6">
+        <v>-0.15263437998935603</v>
       </c>
       <c r="I12" s="6">
-        <v>7.345702139173782E-2</v>
+        <v>-0.10027421904927014</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -965,28 +965,28 @@
         <v>19</v>
       </c>
       <c r="B13" s="3">
-        <v>2181.9400000000005</v>
-      </c>
-      <c r="C13" s="4">
-        <v>-0.25229423818955621</v>
+        <v>2549.5000000000005</v>
+      </c>
+      <c r="C13" s="6">
+        <v>-0.26893961117164622</v>
       </c>
       <c r="D13" s="5">
-        <v>461</v>
-      </c>
-      <c r="E13" s="4">
-        <v>-0.24052718286655683</v>
+        <v>470</v>
+      </c>
+      <c r="E13" s="6">
+        <v>-0.28024502297090348</v>
       </c>
       <c r="F13" s="3">
-        <v>4.7330585683297191</v>
+        <v>5.4244680851063842</v>
       </c>
       <c r="G13" s="4">
-        <v>-1.5493714926378743E-2</v>
-      </c>
-      <c r="H13" s="4">
-        <v>-0.10692930003517409</v>
+        <v>1.5707306180670288E-2</v>
+      </c>
+      <c r="H13" s="6">
+        <v>-0.13894235175510949</v>
       </c>
       <c r="I13" s="4">
-        <v>-0.1873411893573822</v>
+        <v>2.1998935604044645E-2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -994,28 +994,28 @@
         <v>20</v>
       </c>
       <c r="B14" s="3">
-        <v>2918.1799999999994</v>
+        <v>3487.3999999999992</v>
       </c>
       <c r="C14" s="4">
-        <v>-0.33226551219947548</v>
+        <v>4.046518705042379E-2</v>
       </c>
       <c r="D14" s="5">
-        <v>607</v>
+        <v>653</v>
       </c>
       <c r="E14" s="4">
-        <v>-0.33002207505518766</v>
+        <v>1.5337423312884457E-3</v>
       </c>
       <c r="F14" s="3">
-        <v>4.8075453047775936</v>
+        <v>5.3405819295558947</v>
       </c>
       <c r="G14" s="4">
-        <v>-3.3485239748347606E-3</v>
-      </c>
-      <c r="H14" s="4">
-        <v>-0.1403084366495313</v>
-      </c>
-      <c r="I14" s="4">
-        <v>-1.3839611905328564E-3</v>
+        <v>3.8871825355093925E-2</v>
+      </c>
+      <c r="H14" s="6">
+        <v>-3.5616438356164126E-3</v>
+      </c>
+      <c r="I14" s="6">
+        <v>-8.1587510871121705E-2</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1023,28 +1023,28 @@
         <v>21</v>
       </c>
       <c r="B15" s="3">
-        <v>4370.2700000000013</v>
-      </c>
-      <c r="C15" s="4">
-        <v>-0.14371561358684537</v>
+        <v>3351.77</v>
+      </c>
+      <c r="C15" s="6">
+        <v>-3.9973305301991058E-2</v>
       </c>
       <c r="D15" s="5">
-        <v>906</v>
-      </c>
-      <c r="E15" s="4">
-        <v>-0.11867704280155644</v>
+        <v>652</v>
+      </c>
+      <c r="E15" s="6">
+        <v>-4.6783625730994149E-2</v>
       </c>
       <c r="F15" s="3">
-        <v>4.8236975717439305</v>
+        <v>5.1407515337423311</v>
       </c>
       <c r="G15" s="4">
-        <v>-2.8410210559908555E-2</v>
+        <v>7.1445692844143149E-3</v>
       </c>
       <c r="H15" s="6">
-        <v>8.7685830811735213E-2</v>
+        <v>-5.9924450549450503E-2</v>
       </c>
       <c r="I15" s="4">
-        <v>-3.2288849117035889E-2</v>
+        <v>0.2486529680365297</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1052,28 +1052,28 @@
         <v>22</v>
       </c>
       <c r="B16" s="3">
-        <v>5103.7599999999993</v>
-      </c>
-      <c r="C16" s="4">
-        <v>-2.6561027804585802E-2</v>
+        <v>3491.3300000000004</v>
+      </c>
+      <c r="C16" s="6">
+        <v>-7.9894794820911219E-2</v>
       </c>
       <c r="D16" s="5">
-        <v>1028</v>
-      </c>
-      <c r="E16" s="4">
-        <v>-9.6339113680153909E-3</v>
+        <v>684</v>
+      </c>
+      <c r="E16" s="6">
+        <v>-7.1913161465400277E-2</v>
       </c>
       <c r="F16" s="3">
-        <v>4.964747081712062</v>
-      </c>
-      <c r="G16" s="4">
-        <v>-1.7091777102295702E-2</v>
-      </c>
-      <c r="H16" s="4">
-        <v>-6.2299531211448267E-2</v>
+        <v>5.1042836257309947</v>
+      </c>
+      <c r="G16" s="6">
+        <v>-8.6000932500168714E-3</v>
+      </c>
+      <c r="H16" s="6">
+        <v>-4.8366013071895475E-2</v>
       </c>
       <c r="I16" s="6">
-        <v>1.4386264965136064E-2</v>
+        <v>-0.10329670329670326</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1081,28 +1081,28 @@
         <v>23</v>
       </c>
       <c r="B17" s="3">
-        <v>5243.0199999999986</v>
-      </c>
-      <c r="C17" s="6">
-        <v>0.23256131046415399</v>
+        <v>3794.49</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.61785723422217331</v>
       </c>
       <c r="D17" s="5">
-        <v>1038</v>
-      </c>
-      <c r="E17" s="6">
-        <v>0.2783251231527093</v>
+        <v>737</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.59869848156182215</v>
       </c>
       <c r="F17" s="3">
-        <v>5.0510789980732165</v>
+        <v>5.1485617367706915</v>
       </c>
       <c r="G17" s="4">
-        <v>-3.5799822642684886E-2</v>
-      </c>
-      <c r="H17" s="6">
-        <v>0.11506981222917666</v>
+        <v>1.1983968760409747E-2</v>
+      </c>
+      <c r="H17" s="4">
+        <v>4.2944785276073594E-2</v>
       </c>
       <c r="I17" s="4">
-        <v>-0.1209847582541823</v>
+        <v>0.10633484162895934</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1110,28 +1110,28 @@
         <v>24</v>
       </c>
       <c r="B18" s="3">
-        <v>4253.7599999999993</v>
-      </c>
-      <c r="C18" s="6">
-        <v>0.74118918387896959</v>
+        <v>2345.3799999999992</v>
+      </c>
+      <c r="C18" s="4">
+        <v>7.490581775850802E-2</v>
       </c>
       <c r="D18" s="5">
-        <v>812</v>
-      </c>
-      <c r="E18" s="6">
-        <v>0.63052208835341372</v>
+        <v>461</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0</v>
       </c>
       <c r="F18" s="3">
-        <v>5.2386206896551712</v>
-      </c>
-      <c r="G18" s="6">
-        <v>6.7872184201633878E-2</v>
+        <v>5.0875921908893691</v>
+      </c>
+      <c r="G18" s="4">
+        <v>7.490581775850802E-2</v>
       </c>
       <c r="H18" s="6">
-        <v>0.17221639925824395</v>
-      </c>
-      <c r="I18" s="6">
-        <v>0.2104199984604096</v>
+        <v>-7.5541551792044137E-2</v>
+      </c>
+      <c r="I18" s="4">
+        <v>7.345702139173782E-2</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1139,28 +1139,28 @@
         <v>25</v>
       </c>
       <c r="B19" s="3">
-        <v>2443.0199999999995</v>
-      </c>
-      <c r="C19" s="4">
-        <v>-0.16221888438509502</v>
+        <v>2181.94</v>
+      </c>
+      <c r="C19" s="6">
+        <v>-0.25229423818955654</v>
       </c>
       <c r="D19" s="5">
-        <v>498</v>
-      </c>
-      <c r="E19" s="4">
-        <v>-0.15593220338983049</v>
+        <v>461</v>
+      </c>
+      <c r="E19" s="6">
+        <v>-0.24052718286655683</v>
       </c>
       <c r="F19" s="3">
-        <v>4.9056626506024088</v>
-      </c>
-      <c r="G19" s="4">
-        <v>-7.4480758779236211E-3</v>
+        <v>4.7330585683297182</v>
+      </c>
+      <c r="G19" s="6">
+        <v>-1.5493714926379298E-2</v>
       </c>
       <c r="H19" s="6">
-        <v>3.5914140148667784E-2</v>
-      </c>
-      <c r="I19" s="4">
-        <v>-4.5728469948073676E-2</v>
+        <v>-0.10692930003517409</v>
+      </c>
+      <c r="I19" s="6">
+        <v>-0.1873411893573822</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1168,28 +1168,28 @@
         <v>26</v>
       </c>
       <c r="B20" s="3">
-        <v>2916.0599999999995</v>
-      </c>
-      <c r="C20" s="4">
-        <v>-0.27900427495184821</v>
+        <v>2918.1800000000003</v>
+      </c>
+      <c r="C20" s="6">
+        <v>-0.33226551219947514</v>
       </c>
       <c r="D20" s="5">
-        <v>590</v>
-      </c>
-      <c r="E20" s="4">
-        <v>-0.25786163522012584</v>
+        <v>607</v>
+      </c>
+      <c r="E20" s="6">
+        <v>-0.33002207505518766</v>
       </c>
       <c r="F20" s="3">
-        <v>4.9424745762711852</v>
-      </c>
-      <c r="G20" s="4">
-        <v>-2.8488811163931205E-2</v>
-      </c>
-      <c r="H20" s="4">
-        <v>-6.3900414937759775E-3</v>
-      </c>
-      <c r="I20" s="4">
-        <v>-0.2126383808725415</v>
+        <v>4.8075453047775953</v>
+      </c>
+      <c r="G20" s="6">
+        <v>-3.3485239748344275E-3</v>
+      </c>
+      <c r="H20" s="6">
+        <v>-0.1403084366495313</v>
+      </c>
+      <c r="I20" s="6">
+        <v>-1.3839611905328564E-3</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1197,28 +1197,28 @@
         <v>27</v>
       </c>
       <c r="B21" s="3">
-        <v>4044.4900000000002</v>
-      </c>
-      <c r="C21" s="4">
-        <v>-0.19227804316914576</v>
+        <v>4370.2700000000013</v>
+      </c>
+      <c r="C21" s="6">
+        <v>-0.1437156135868457</v>
       </c>
       <c r="D21" s="5">
-        <v>795</v>
-      </c>
-      <c r="E21" s="4">
-        <v>-0.19858870967741937</v>
+        <v>906</v>
+      </c>
+      <c r="E21" s="6">
+        <v>-0.11867704280155644</v>
       </c>
       <c r="F21" s="3">
-        <v>5.0874088050314468</v>
+        <v>4.8236975717439305</v>
       </c>
       <c r="G21" s="6">
-        <v>7.8744417310783188E-3</v>
+        <v>-2.8410210559908777E-2</v>
       </c>
       <c r="H21" s="4">
-        <v>-0.111684482123111</v>
+        <v>8.7685830811735213E-2</v>
       </c>
       <c r="I21" s="6">
-        <v>6.3110176762481984E-2</v>
+        <v>-3.2288849117035889E-2</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1226,28 +1226,28 @@
         <v>28</v>
       </c>
       <c r="B22" s="3">
-        <v>5007.28</v>
-      </c>
-      <c r="C22" s="4">
-        <v>-4.4443214628532617E-2</v>
+        <v>5103.7600000000011</v>
+      </c>
+      <c r="C22" s="6">
+        <v>-2.6561027804585802E-2</v>
       </c>
       <c r="D22" s="5">
-        <v>992</v>
-      </c>
-      <c r="E22" s="4">
-        <v>-3.9690222652468576E-2</v>
+        <v>1028</v>
+      </c>
+      <c r="E22" s="6">
+        <v>-9.6339113680153909E-3</v>
       </c>
       <c r="F22" s="3">
-        <v>5.0476612903225808</v>
-      </c>
-      <c r="G22" s="4">
-        <v>-4.9494362008811743E-3</v>
-      </c>
-      <c r="H22" s="4">
-        <v>-5.4176544415004857E-2</v>
-      </c>
-      <c r="I22" s="6">
-        <v>1.7893323527001348E-2</v>
+        <v>4.9647470817120629</v>
+      </c>
+      <c r="G22" s="6">
+        <v>-1.7091777102295813E-2</v>
+      </c>
+      <c r="H22" s="6">
+        <v>-6.2299531211448267E-2</v>
+      </c>
+      <c r="I22" s="4">
+        <v>1.4386264965136064E-2</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -1255,28 +1255,28 @@
         <v>29</v>
       </c>
       <c r="B23" s="3">
-        <v>5240.1699999999973</v>
-      </c>
-      <c r="C23" s="6">
-        <v>0.16124364272972039</v>
+        <v>5243.02</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.23256131046415374</v>
       </c>
       <c r="D23" s="5">
-        <v>1033</v>
-      </c>
-      <c r="E23" s="6">
-        <v>0.12404787812840044</v>
+        <v>1038</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.2783251231527093</v>
       </c>
       <c r="F23" s="3">
-        <v>5.0727686350435599</v>
+        <v>5.0510789980732183</v>
       </c>
       <c r="G23" s="6">
-        <v>3.3090907714049322E-2</v>
-      </c>
-      <c r="H23" s="6">
-        <v>2.0637631653857014E-2</v>
+        <v>-3.5799822642684997E-2</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0.11506981222917666</v>
       </c>
       <c r="I23" s="6">
-        <v>5.53253871502557E-3</v>
+        <v>-0.1209847582541823</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -1284,28 +1284,28 @@
         <v>30</v>
       </c>
       <c r="B24" s="3">
-        <v>4512.5499999999984</v>
+        <v>4253.7600000000011</v>
       </c>
       <c r="C24" s="4">
-        <v>-6.2635020606222058E-2</v>
+        <v>0.7411891838789697</v>
       </c>
       <c r="D24" s="5">
-        <v>919</v>
+        <v>812</v>
       </c>
       <c r="E24" s="4">
-        <v>-1.076426264800856E-2</v>
+        <v>0.63052208835341372</v>
       </c>
       <c r="F24" s="3">
-        <v>4.9102829162132737</v>
+        <v>5.2386206896551739</v>
       </c>
       <c r="G24" s="4">
-        <v>-5.2435184051338728E-2</v>
-      </c>
-      <c r="H24" s="6">
-        <v>1.8556103218324127E-2</v>
+        <v>6.78721842016341E-2</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0.17221639925824395</v>
       </c>
       <c r="I24" s="4">
-        <v>-3.9375824858318698E-3</v>
+        <v>0.2104199984604096</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -1313,28 +1313,28 @@
         <v>31</v>
       </c>
       <c r="B25" s="3">
-        <v>4814.08</v>
+        <v>2443.0200000000004</v>
       </c>
       <c r="C25" s="6">
-        <v>0.71975036527119429</v>
+        <v>-0.16221888438509513</v>
       </c>
       <c r="D25" s="5">
-        <v>929</v>
+        <v>498</v>
       </c>
       <c r="E25" s="6">
-        <v>0.58262350936967633</v>
+        <v>-0.15593220338983049</v>
       </c>
       <c r="F25" s="3">
-        <v>5.1820021528525295</v>
+        <v>4.9056626506024106</v>
       </c>
       <c r="G25" s="6">
-        <v>8.6645279240248771E-2</v>
-      </c>
-      <c r="H25" s="6">
-        <v>0.53904506916555106</v>
+        <v>-7.4480758779240652E-3</v>
+      </c>
+      <c r="H25" s="4">
+        <v>3.5914140148667784E-2</v>
       </c>
       <c r="I25" s="6">
-        <v>3.832734451607811E-3</v>
+        <v>-4.5728469948073676E-2</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -1342,28 +1342,28 @@
         <v>32</v>
       </c>
       <c r="B26" s="3">
-        <v>2799.2899999999991</v>
+        <v>2916.0600000000013</v>
       </c>
       <c r="C26" s="6">
-        <v>1.2518627833961959E-2</v>
+        <v>-0.27900427495184754</v>
       </c>
       <c r="D26" s="5">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="E26" s="6">
-        <v>2.8021015761821255E-2</v>
+        <v>-0.25786163522012584</v>
       </c>
       <c r="F26" s="3">
-        <v>4.7688074957410542</v>
-      </c>
-      <c r="G26" s="4">
-        <v>-1.5079835616367609E-2</v>
-      </c>
-      <c r="H26" s="4">
-        <v>-9.9638408999598194E-2</v>
-      </c>
-      <c r="I26" s="4">
-        <v>-3.0890446316857889E-2</v>
+        <v>4.9424745762711888</v>
+      </c>
+      <c r="G26" s="6">
+        <v>-2.8488811163930094E-2</v>
+      </c>
+      <c r="H26" s="6">
+        <v>-6.3900414937759775E-3</v>
+      </c>
+      <c r="I26" s="6">
+        <v>-0.2126383808725415</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1371,28 +1371,28 @@
         <v>33</v>
       </c>
       <c r="B27" s="3">
-        <v>2764.6800000000012</v>
+        <v>4044.4899999999989</v>
       </c>
       <c r="C27" s="6">
-        <v>9.5855877281646004E-2</v>
+        <v>-0.19227804316914632</v>
       </c>
       <c r="D27" s="5">
-        <v>571</v>
+        <v>795</v>
       </c>
       <c r="E27" s="6">
-        <v>0.13069306930693059</v>
+        <v>-0.19858870967741937</v>
       </c>
       <c r="F27" s="3">
-        <v>4.8418213660245204</v>
+        <v>5.087408805031445</v>
       </c>
       <c r="G27" s="4">
-        <v>-3.081047630957745E-2</v>
-      </c>
-      <c r="H27" s="4">
-        <v>-0.24242885405569925</v>
-      </c>
-      <c r="I27" s="6">
-        <v>6.2953838996849365E-2</v>
+        <v>7.8744417310776527E-3</v>
+      </c>
+      <c r="H27" s="6">
+        <v>-0.111684482123111</v>
+      </c>
+      <c r="I27" s="4">
+        <v>6.3110176762481984E-2</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1400,28 +1400,28 @@
         <v>34</v>
       </c>
       <c r="B28" s="3">
-        <v>2522.8500000000004</v>
-      </c>
-      <c r="C28" s="4">
-        <v>-0.42443392459932694</v>
+        <v>5007.2800000000025</v>
+      </c>
+      <c r="C28" s="6">
+        <v>-4.4443214628532735E-2</v>
       </c>
       <c r="D28" s="5">
-        <v>505</v>
-      </c>
-      <c r="E28" s="4">
-        <v>-0.4363839285714286</v>
+        <v>992</v>
+      </c>
+      <c r="E28" s="6">
+        <v>-3.9690222652468576E-2</v>
       </c>
       <c r="F28" s="3">
-        <v>4.9957425742574264</v>
+        <v>5.0476612903225835</v>
       </c>
       <c r="G28" s="6">
-        <v>2.1202383285154669E-2</v>
-      </c>
-      <c r="H28" s="4">
-        <v>-8.2582897033158797E-2</v>
-      </c>
-      <c r="I28" s="6">
-        <v>2.3995948787222776E-2</v>
+        <v>-4.9494362008812853E-3</v>
+      </c>
+      <c r="H28" s="6">
+        <v>-5.4176544415004857E-2</v>
+      </c>
+      <c r="I28" s="4">
+        <v>1.7893323527001348E-2</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1429,28 +1429,28 @@
         <v>35</v>
       </c>
       <c r="B29" s="3">
-        <v>4383.25</v>
+        <v>5240.170000000001</v>
       </c>
       <c r="C29" s="4">
-        <v>-0.22422825467507224</v>
+        <v>0.1612436427297208</v>
       </c>
       <c r="D29" s="5">
-        <v>896</v>
+        <v>1033</v>
       </c>
       <c r="E29" s="4">
-        <v>-0.25020920502092048</v>
+        <v>0.12404787812840044</v>
       </c>
       <c r="F29" s="3">
-        <v>4.8920200892857144</v>
-      </c>
-      <c r="G29" s="6">
-        <v>3.4650932659920475E-2</v>
+        <v>5.0727686350435635</v>
+      </c>
+      <c r="G29" s="4">
+        <v>3.3090907714049766E-2</v>
       </c>
       <c r="H29" s="4">
-        <v>-0.10013191783403486</v>
+        <v>2.0637631653857014E-2</v>
       </c>
       <c r="I29" s="4">
-        <v>-0.16602906940977247</v>
+        <v>5.53253871502557E-3</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -1458,28 +1458,28 @@
         <v>36</v>
       </c>
       <c r="B30" s="3">
-        <v>5650.1799999999994</v>
+        <v>4512.5499999999993</v>
       </c>
       <c r="C30" s="6">
-        <v>2.5297735162236989E-2</v>
+        <v>-6.2635020606221836E-2</v>
       </c>
       <c r="D30" s="5">
-        <v>1195</v>
+        <v>919</v>
       </c>
       <c r="E30" s="6">
-        <v>4.2016806722688926E-3</v>
+        <v>-1.076426264800856E-2</v>
       </c>
       <c r="F30" s="3">
-        <v>4.7281841004184093</v>
+        <v>4.9102829162132746</v>
       </c>
       <c r="G30" s="6">
-        <v>2.1007786479549706E-2</v>
+        <v>-5.243518405133852E-2</v>
       </c>
       <c r="H30" s="4">
-        <v>-2.7372151280014689E-2</v>
+        <v>1.8556103218324127E-2</v>
       </c>
       <c r="I30" s="6">
-        <v>3.8741878180971634E-2</v>
+        <v>-3.9375824858318698E-3</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -1487,28 +1487,28 @@
         <v>37</v>
       </c>
       <c r="B31" s="3">
-        <v>5510.7699999999986</v>
-      </c>
-      <c r="C31" s="6">
-        <v>0.11299906286859172</v>
+        <v>4814.08</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.71975036527119429</v>
       </c>
       <c r="D31" s="5">
-        <v>1190</v>
-      </c>
-      <c r="E31" s="6">
-        <v>0.1531007751937985</v>
+        <v>929</v>
+      </c>
+      <c r="E31" s="4">
+        <v>0.58262350936967633</v>
       </c>
       <c r="F31" s="3">
-        <v>4.6308991596638647</v>
+        <v>5.1820021528525295</v>
       </c>
       <c r="G31" s="4">
-        <v>-3.4777283293792705E-2</v>
+        <v>8.6645279240248771E-2</v>
       </c>
       <c r="H31" s="4">
-        <v>-7.9212376933895934E-2</v>
+        <v>0.53904506916555106</v>
       </c>
       <c r="I31" s="4">
-        <v>-1.9635740978116489E-2</v>
+        <v>3.832734451607811E-3</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -1516,28 +1516,28 @@
         <v>38</v>
       </c>
       <c r="B32" s="3">
-        <v>4951.2799999999979</v>
-      </c>
-      <c r="C32" s="6">
-        <v>0.67158898319390015</v>
+        <v>2799.2899999999991</v>
+      </c>
+      <c r="C32" s="4">
+        <v>1.2518627833962404E-2</v>
       </c>
       <c r="D32" s="5">
-        <v>1032</v>
-      </c>
-      <c r="E32" s="6">
-        <v>0.68352365415986949</v>
+        <v>587</v>
+      </c>
+      <c r="E32" s="4">
+        <v>2.8021015761821255E-2</v>
       </c>
       <c r="F32" s="3">
-        <v>4.7977519379844944</v>
-      </c>
-      <c r="G32" s="4">
-        <v>-7.0891020369564517E-3</v>
+        <v>4.7688074957410542</v>
+      </c>
+      <c r="G32" s="6">
+        <v>-1.5079835616367054E-2</v>
       </c>
       <c r="H32" s="6">
-        <v>0.44500447118120467</v>
+        <v>-9.9638408999598194E-2</v>
       </c>
       <c r="I32" s="6">
-        <v>0.17527377661380286</v>
+        <v>-3.0890446316857889E-2</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -1545,28 +1545,28 @@
         <v>39</v>
       </c>
       <c r="B33" s="3">
-        <v>2962.0200000000009</v>
-      </c>
-      <c r="C33" s="6">
-        <v>1.3779365861672721E-2</v>
+        <v>2764.68</v>
+      </c>
+      <c r="C33" s="4">
+        <v>9.5855877281645352E-2</v>
       </c>
       <c r="D33" s="5">
-        <v>613</v>
+        <v>571</v>
       </c>
       <c r="E33" s="4">
-        <v>-1.7628205128205177E-2</v>
+        <v>0.13069306930693059</v>
       </c>
       <c r="F33" s="3">
-        <v>4.8320065252854825</v>
+        <v>4.8418213660245177</v>
       </c>
       <c r="G33" s="6">
-        <v>3.1971165249076394E-2</v>
-      </c>
-      <c r="H33" s="4">
-        <v>-5.500499347007759E-2</v>
-      </c>
-      <c r="I33" s="6">
-        <v>4.9162148584959819E-2</v>
+        <v>-3.0810476309578227E-2</v>
+      </c>
+      <c r="H33" s="6">
+        <v>-0.24242885405569925</v>
+      </c>
+      <c r="I33" s="4">
+        <v>6.2953838996849365E-2</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -1574,28 +1574,28 @@
         <v>40</v>
       </c>
       <c r="B34" s="3">
-        <v>2921.7599999999998</v>
-      </c>
-      <c r="C34" s="4">
-        <v>-0.46721129123434063</v>
+        <v>2522.8500000000008</v>
+      </c>
+      <c r="C34" s="6">
+        <v>-0.42443392459932694</v>
       </c>
       <c r="D34" s="5">
-        <v>624</v>
-      </c>
-      <c r="E34" s="4">
-        <v>-0.43631436314363148</v>
+        <v>505</v>
+      </c>
+      <c r="E34" s="6">
+        <v>-0.4363839285714286</v>
       </c>
       <c r="F34" s="3">
-        <v>4.6823076923076918</v>
+        <v>4.9957425742574273</v>
       </c>
       <c r="G34" s="4">
-        <v>-5.4812338776306202E-2</v>
-      </c>
-      <c r="H34" s="4">
-        <v>-0.13219999999999998</v>
+        <v>2.1202383285154669E-2</v>
+      </c>
+      <c r="H34" s="6">
+        <v>-8.2582897033158797E-2</v>
       </c>
       <c r="I34" s="4">
-        <v>-0.13942324194711009</v>
+        <v>2.3995948787222776E-2</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1603,28 +1603,28 @@
         <v>41</v>
       </c>
       <c r="B35" s="3">
-        <v>5483.9000000000005</v>
-      </c>
-      <c r="C35" s="4">
-        <v>-0.27704347046555311</v>
+        <v>4383.2500000000018</v>
+      </c>
+      <c r="C35" s="6">
+        <v>-0.22422825467507168</v>
       </c>
       <c r="D35" s="5">
-        <v>1107</v>
-      </c>
-      <c r="E35" s="4">
-        <v>-0.30725907384230289</v>
+        <v>896</v>
+      </c>
+      <c r="E35" s="6">
+        <v>-0.25020920502092048</v>
       </c>
       <c r="F35" s="3">
-        <v>4.9538392050587179</v>
-      </c>
-      <c r="G35" s="6">
-        <v>4.36174653984156E-2</v>
-      </c>
-      <c r="H35" s="4">
-        <v>-0.13703831549879186</v>
+        <v>4.8920200892857162</v>
+      </c>
+      <c r="G35" s="4">
+        <v>3.4650932659921141E-2</v>
+      </c>
+      <c r="H35" s="6">
+        <v>-0.10013191783403486</v>
       </c>
       <c r="I35" s="6">
-        <v>1.1691176470587372E-3</v>
+        <v>-0.16602906940977247</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -1632,28 +1632,28 @@
         <v>42</v>
       </c>
       <c r="B36" s="3">
-        <v>7585.3799999999965</v>
-      </c>
-      <c r="C36" s="6">
-        <v>0.67100202228478478</v>
+        <v>5650.1799999999976</v>
+      </c>
+      <c r="C36" s="4">
+        <v>2.5297735162236323E-2</v>
       </c>
       <c r="D36" s="5">
-        <v>1598</v>
-      </c>
-      <c r="E36" s="6">
-        <v>0.87999999999999989</v>
+        <v>1195</v>
+      </c>
+      <c r="E36" s="4">
+        <v>4.2016806722688926E-3</v>
       </c>
       <c r="F36" s="3">
-        <v>4.7467959949937404</v>
+        <v>4.7281841004184084</v>
       </c>
       <c r="G36" s="4">
-        <v>-0.11116913708256126</v>
-      </c>
-      <c r="H36" s="4">
-        <v>-5.8753452103752594E-2</v>
+        <v>2.1007786479549262E-2</v>
+      </c>
+      <c r="H36" s="6">
+        <v>-2.7372151280014689E-2</v>
       </c>
       <c r="I36" s="4">
-        <v>-2.7008473102133168E-2</v>
+        <v>3.8741878180971634E-2</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -1661,28 +1661,28 @@
         <v>43</v>
       </c>
       <c r="B37" s="3">
-        <v>4539.4199999999992</v>
-      </c>
-      <c r="C37" s="6">
-        <v>1.3239748118568562</v>
+        <v>5510.77</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0.11299906286859196</v>
       </c>
       <c r="D37" s="5">
-        <v>850</v>
-      </c>
-      <c r="E37" s="6">
-        <v>1.5914634146341462</v>
+        <v>1190</v>
+      </c>
+      <c r="E37" s="4">
+        <v>0.1531007751937985</v>
       </c>
       <c r="F37" s="3">
-        <v>5.3404941176470579</v>
-      </c>
-      <c r="G37" s="4">
-        <v>-0.10321913142464843</v>
+        <v>4.6308991596638656</v>
+      </c>
+      <c r="G37" s="6">
+        <v>-3.4777283293792705E-2</v>
       </c>
       <c r="H37" s="6">
-        <v>0.2116659011875861</v>
+        <v>-7.9212376933895934E-2</v>
       </c>
       <c r="I37" s="6">
-        <v>1.1222257463119543</v>
+        <v>-1.9635740978116489E-2</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -1690,28 +1690,28 @@
         <v>44</v>
       </c>
       <c r="B38" s="3">
-        <v>1953.3000000000009</v>
+        <v>4951.2799999999988</v>
       </c>
       <c r="C38" s="4">
-        <v>-8.970588920630608E-2</v>
+        <v>0.67158898319390081</v>
       </c>
       <c r="D38" s="5">
-        <v>328</v>
+        <v>1032</v>
       </c>
       <c r="E38" s="4">
-        <v>-7.8651685393258397E-2</v>
+        <v>0.68352365415986949</v>
       </c>
       <c r="F38" s="3">
-        <v>5.9551829268292709</v>
-      </c>
-      <c r="G38" s="4">
-        <v>-1.1997855358063858E-2</v>
-      </c>
-      <c r="H38" s="6">
-        <v>3.4129461256615645E-2</v>
-      </c>
-      <c r="I38" s="6">
-        <v>0.17257893776990899</v>
+        <v>4.7977519379844953</v>
+      </c>
+      <c r="G38" s="6">
+        <v>-7.0891020369560076E-3</v>
+      </c>
+      <c r="H38" s="4">
+        <v>0.44500447118120467</v>
+      </c>
+      <c r="I38" s="4">
+        <v>0.17527377661380286</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -1719,28 +1719,28 @@
         <v>45</v>
       </c>
       <c r="B39" s="3">
-        <v>2145.7900000000004</v>
-      </c>
-      <c r="C39" s="6">
-        <v>0.41808533135953962</v>
+        <v>2962.0200000000004</v>
+      </c>
+      <c r="C39" s="4">
+        <v>1.3779365861672499E-2</v>
       </c>
       <c r="D39" s="5">
-        <v>356</v>
+        <v>613</v>
       </c>
       <c r="E39" s="6">
-        <v>0.42971887550200805</v>
+        <v>-1.7628205128205177E-2</v>
       </c>
       <c r="F39" s="3">
-        <v>6.0275000000000007</v>
+        <v>4.8320065252854816</v>
       </c>
       <c r="G39" s="4">
-        <v>-8.1369452007714616E-3</v>
+        <v>3.197116524907595E-2</v>
       </c>
       <c r="H39" s="6">
-        <v>0.35809067453004045</v>
-      </c>
-      <c r="I39" s="6">
-        <v>6.6695492936961864E-2</v>
+        <v>-5.500499347007759E-2</v>
+      </c>
+      <c r="I39" s="4">
+        <v>4.9162148584959819E-2</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -1748,28 +1748,28 @@
         <v>46</v>
       </c>
       <c r="B40" s="3">
-        <v>1513.1599999999996</v>
+        <v>2921.76</v>
       </c>
       <c r="C40" s="6">
-        <v>8.992163190042636E-2</v>
+        <v>-0.46721129123434046</v>
       </c>
       <c r="D40" s="5">
-        <v>249</v>
+        <v>624</v>
       </c>
       <c r="E40" s="6">
-        <v>0.14746543778801846</v>
+        <v>-0.43631436314363148</v>
       </c>
       <c r="F40" s="3">
-        <v>6.076947791164657</v>
-      </c>
-      <c r="G40" s="4">
-        <v>-5.0148617982359485E-2</v>
-      </c>
-      <c r="H40" s="4">
-        <v>-4.8987818771360929E-2</v>
-      </c>
-      <c r="I40" s="4">
-        <v>-6.5718051722935655E-2</v>
+        <v>4.6823076923076927</v>
+      </c>
+      <c r="G40" s="6">
+        <v>-5.4812338776305862E-2</v>
+      </c>
+      <c r="H40" s="6">
+        <v>-0.13219999999999998</v>
+      </c>
+      <c r="I40" s="6">
+        <v>-0.13942324194711009</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -1777,28 +1777,28 @@
         <v>47</v>
       </c>
       <c r="B41" s="3">
-        <v>1388.3199999999997</v>
-      </c>
-      <c r="C41" s="4">
-        <v>-0.51067076931752908</v>
+        <v>5483.9</v>
+      </c>
+      <c r="C41" s="6">
+        <v>-0.27704347046555344</v>
       </c>
       <c r="D41" s="5">
-        <v>217</v>
-      </c>
-      <c r="E41" s="4">
-        <v>-0.54507337526205446</v>
+        <v>1107</v>
+      </c>
+      <c r="E41" s="6">
+        <v>-0.30725907384230289</v>
       </c>
       <c r="F41" s="3">
-        <v>6.3977880184331788</v>
-      </c>
-      <c r="G41" s="6">
-        <v>7.5622318136122635E-2</v>
-      </c>
-      <c r="H41" s="4">
-        <v>-7.7675396055609469E-2</v>
+        <v>4.953839205058717</v>
+      </c>
+      <c r="G41" s="4">
+        <v>4.3617465398415378E-2</v>
+      </c>
+      <c r="H41" s="6">
+        <v>-0.13703831549879186</v>
       </c>
       <c r="I41" s="4">
-        <v>-9.8516215872915827E-2</v>
+        <v>1.1691176470587372E-3</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
@@ -1806,28 +1806,28 @@
         <v>48</v>
       </c>
       <c r="B42" s="3">
-        <v>2837.19</v>
+        <v>7585.3799999999992</v>
       </c>
       <c r="C42" s="4">
-        <v>-0.37734904962658772</v>
+        <v>0.67100202228478489</v>
       </c>
       <c r="D42" s="5">
-        <v>477</v>
+        <v>1598</v>
       </c>
       <c r="E42" s="4">
-        <v>-0.38610038610038605</v>
+        <v>0.87999999999999989</v>
       </c>
       <c r="F42" s="3">
-        <v>5.9479874213836483</v>
+        <v>4.7467959949937413</v>
       </c>
       <c r="G42" s="6">
-        <v>1.4255321677445032E-2</v>
-      </c>
-      <c r="H42" s="4">
-        <v>-0.20595597201720039</v>
-      </c>
-      <c r="I42" s="4">
-        <v>-0.19796447283871998</v>
+        <v>-0.11116913708256115</v>
+      </c>
+      <c r="H42" s="6">
+        <v>-5.8753452103752594E-2</v>
+      </c>
+      <c r="I42" s="6">
+        <v>-2.7008473102133168E-2</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
@@ -1835,28 +1835,28 @@
         <v>49</v>
       </c>
       <c r="B43" s="3">
-        <v>4556.6299999999983</v>
+        <v>4539.42</v>
       </c>
       <c r="C43" s="4">
-        <v>-0.1837126979975422</v>
+        <v>1.3239748118568564</v>
       </c>
       <c r="D43" s="5">
-        <v>777</v>
+        <v>850</v>
       </c>
       <c r="E43" s="4">
-        <v>-0.22686567164179106</v>
+        <v>1.5914634146341462</v>
       </c>
       <c r="F43" s="3">
-        <v>5.864388674388672</v>
+        <v>5.3404941176470588</v>
       </c>
       <c r="G43" s="6">
-        <v>5.5815622281171207E-2</v>
+        <v>-0.10321913142464822</v>
       </c>
       <c r="H43" s="4">
-        <v>-0.2217282717282717</v>
+        <v>0.2116659011875861</v>
       </c>
       <c r="I43" s="4">
-        <v>-0.11761899888464289</v>
+        <v>1.1222257463119543</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -1864,28 +1864,28 @@
         <v>50</v>
       </c>
       <c r="B44" s="3">
-        <v>5582.1399999999985</v>
+        <v>1953.3000000000006</v>
       </c>
       <c r="C44" s="6">
-        <v>8.5542154616841545E-2</v>
+        <v>-8.9705889206305955E-2</v>
       </c>
       <c r="D44" s="5">
-        <v>1005</v>
+        <v>328</v>
       </c>
       <c r="E44" s="6">
-        <v>8.6486486486486491E-2</v>
+        <v>-7.8651685393258397E-2</v>
       </c>
       <c r="F44" s="3">
-        <v>5.5543681592039782</v>
-      </c>
-      <c r="G44" s="4">
-        <v>-8.6916117355384515E-4</v>
-      </c>
-      <c r="H44" s="6">
-        <v>8.6508194941929961E-2</v>
+        <v>5.95518292682927</v>
+      </c>
+      <c r="G44" s="6">
+        <v>-1.1997855358063858E-2</v>
+      </c>
+      <c r="H44" s="4">
+        <v>3.4129461256615645E-2</v>
       </c>
       <c r="I44" s="4">
-        <v>-0.22444201760971949</v>
+        <v>0.17257893776990899</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -1893,28 +1893,28 @@
         <v>51</v>
       </c>
       <c r="B45" s="3">
-        <v>5142.2599999999993</v>
-      </c>
-      <c r="C45" s="6">
-        <v>0.21350982062579216</v>
+        <v>2145.79</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0.41808533135953874</v>
       </c>
       <c r="D45" s="5">
-        <v>925</v>
-      </c>
-      <c r="E45" s="6">
-        <v>0.17684478371501267</v>
+        <v>356</v>
+      </c>
+      <c r="E45" s="4">
+        <v>0.42971887550200805</v>
       </c>
       <c r="F45" s="3">
-        <v>5.5591999999999988</v>
+        <v>6.0274999999999999</v>
       </c>
       <c r="G45" s="6">
-        <v>3.1155371904727058E-2</v>
-      </c>
-      <c r="H45" s="6">
-        <v>0.28898216159496326</v>
+        <v>-8.1369452007721277E-3</v>
+      </c>
+      <c r="H45" s="4">
+        <v>0.35809067453004045</v>
       </c>
       <c r="I45" s="4">
-        <v>-1.6497998805180325E-2</v>
+        <v>6.6695492936961864E-2</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
@@ -1922,28 +1922,28 @@
         <v>52</v>
       </c>
       <c r="B46" s="3">
-        <v>4237.5099999999993</v>
-      </c>
-      <c r="C46" s="6">
-        <v>1.1938618608046472</v>
+        <v>1513.1600000000003</v>
+      </c>
+      <c r="C46" s="4">
+        <v>8.9921631900426777E-2</v>
       </c>
       <c r="D46" s="5">
-        <v>786</v>
-      </c>
-      <c r="E46" s="6">
-        <v>1.0793650793650795</v>
+        <v>249</v>
+      </c>
+      <c r="E46" s="4">
+        <v>0.14746543778801846</v>
       </c>
       <c r="F46" s="3">
-        <v>5.3912340966921111</v>
+        <v>6.0769477911646597</v>
       </c>
       <c r="G46" s="6">
-        <v>5.5063337638876275E-2</v>
+        <v>-5.0148617982359145E-2</v>
       </c>
       <c r="H46" s="6">
-        <v>0.41045880611741481</v>
+        <v>-4.8987818771360929E-2</v>
       </c>
       <c r="I46" s="6">
-        <v>3.4961183276847052E-2</v>
+        <v>-6.5718051722935655E-2</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
@@ -1951,28 +1951,28 @@
         <v>53</v>
       </c>
       <c r="B47" s="3">
-        <v>1931.5299999999995</v>
+        <v>1388.3199999999997</v>
       </c>
       <c r="C47" s="6">
-        <v>2.7316678810958228E-2</v>
+        <v>-0.51067076931752908</v>
       </c>
       <c r="D47" s="5">
-        <v>378</v>
+        <v>217</v>
       </c>
       <c r="E47" s="6">
-        <v>0.10850439882697938</v>
+        <v>-0.54507337526205446</v>
       </c>
       <c r="F47" s="3">
-        <v>5.1098677248677236</v>
+        <v>6.3977880184331788</v>
       </c>
       <c r="G47" s="4">
-        <v>-7.3240773876886989E-2</v>
-      </c>
-      <c r="H47" s="4">
-        <v>-3.171873507213141E-2</v>
-      </c>
-      <c r="I47" s="4">
-        <v>-8.6271938993084843E-2</v>
+        <v>7.5622318136122635E-2</v>
+      </c>
+      <c r="H47" s="6">
+        <v>-7.7675396055609469E-2</v>
+      </c>
+      <c r="I47" s="6">
+        <v>-9.8516215872915827E-2</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
@@ -1980,28 +1980,28 @@
         <v>54</v>
       </c>
       <c r="B48" s="3">
-        <v>1880.1700000000003</v>
-      </c>
-      <c r="C48" s="4">
-        <v>-7.6523720879973722E-2</v>
+        <v>2837.19</v>
+      </c>
+      <c r="C48" s="6">
+        <v>-0.37734904962658766</v>
       </c>
       <c r="D48" s="5">
-        <v>341</v>
-      </c>
-      <c r="E48" s="4">
-        <v>-6.0606060606060552E-2</v>
+        <v>477</v>
+      </c>
+      <c r="E48" s="6">
+        <v>-0.38610038610038605</v>
       </c>
       <c r="F48" s="3">
-        <v>5.5136950146627575</v>
+        <v>5.9479874213836483</v>
       </c>
       <c r="G48" s="4">
-        <v>-1.6944606098036497E-2</v>
+        <v>1.4255321677445254E-2</v>
       </c>
       <c r="H48" s="6">
-        <v>1.3164262898073709E-2</v>
-      </c>
-      <c r="I48" s="4">
-        <v>-6.6772432529096371E-2</v>
+        <v>-0.20595597201720039</v>
+      </c>
+      <c r="I48" s="6">
+        <v>-0.19796447283871998</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
@@ -2009,28 +2009,28 @@
         <v>55</v>
       </c>
       <c r="B49" s="3">
-        <v>2035.9700000000005</v>
-      </c>
-      <c r="C49" s="4">
-        <v>-0.10456432630227031</v>
+        <v>4556.6299999999974</v>
+      </c>
+      <c r="C49" s="6">
+        <v>-0.18371269799754253</v>
       </c>
       <c r="D49" s="5">
-        <v>363</v>
-      </c>
-      <c r="E49" s="4">
-        <v>-0.17123287671232881</v>
+        <v>777</v>
+      </c>
+      <c r="E49" s="6">
+        <v>-0.22686567164179106</v>
       </c>
       <c r="F49" s="3">
-        <v>5.6087327823691471</v>
-      </c>
-      <c r="G49" s="6">
-        <v>8.0443044296434105E-2</v>
-      </c>
-      <c r="H49" s="4">
-        <v>-0.10939655172413797</v>
+        <v>5.8643886743886711</v>
+      </c>
+      <c r="G49" s="4">
+        <v>5.5815622281170985E-2</v>
+      </c>
+      <c r="H49" s="6">
+        <v>-0.2217282717282717</v>
       </c>
       <c r="I49" s="6">
-        <v>0.30962342717725533</v>
+        <v>-0.11761899888464289</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
@@ -2038,28 +2038,28 @@
         <v>56</v>
       </c>
       <c r="B50" s="3">
-        <v>2273.7199999999984</v>
+        <v>5582.1399999999994</v>
       </c>
       <c r="C50" s="4">
-        <v>-0.29984880537772507</v>
+        <v>8.5542154616841545E-2</v>
       </c>
       <c r="D50" s="5">
-        <v>438</v>
+        <v>1005</v>
       </c>
       <c r="E50" s="4">
-        <v>-0.22751322751322756</v>
+        <v>8.6486486486486491E-2</v>
       </c>
       <c r="F50" s="3">
-        <v>5.1911415525114117</v>
-      </c>
-      <c r="G50" s="4">
-        <v>-9.3639891893082527E-2</v>
+        <v>5.5543681592039791</v>
+      </c>
+      <c r="G50" s="6">
+        <v>-8.6916117355373412E-4</v>
       </c>
       <c r="H50" s="4">
-        <v>-4.5188904436579191E-2</v>
-      </c>
-      <c r="I50" s="4">
-        <v>-3.3930588585017851E-2</v>
+        <v>8.6508194941929961E-2</v>
+      </c>
+      <c r="I50" s="6">
+        <v>-0.22444201760971949</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -2067,28 +2067,28 @@
         <v>57</v>
       </c>
       <c r="B51" s="3">
-        <v>3247.4699999999989</v>
+        <v>5142.2599999999993</v>
       </c>
       <c r="C51" s="4">
-        <v>-0.35253773658260401</v>
+        <v>0.21350982062579216</v>
       </c>
       <c r="D51" s="5">
-        <v>567</v>
+        <v>925</v>
       </c>
       <c r="E51" s="4">
-        <v>-0.38503253796095449</v>
+        <v>0.17684478371501267</v>
       </c>
       <c r="F51" s="3">
-        <v>5.7274603174603156</v>
-      </c>
-      <c r="G51" s="6">
-        <v>5.283987102440757E-2</v>
+        <v>5.5591999999999988</v>
+      </c>
+      <c r="G51" s="4">
+        <v>3.1155371904727058E-2</v>
       </c>
       <c r="H51" s="4">
-        <v>-0.14845447536272516</v>
-      </c>
-      <c r="I51" s="4">
-        <v>-6.4403166181090321E-2</v>
+        <v>0.28898216159496326</v>
+      </c>
+      <c r="I51" s="6">
+        <v>-1.6497998805180325E-2</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
@@ -2096,28 +2096,28 @@
         <v>58</v>
       </c>
       <c r="B52" s="3">
-        <v>5015.6899999999996</v>
-      </c>
-      <c r="C52" s="6">
-        <v>4.6650909382257577E-3</v>
+        <v>4237.5099999999993</v>
+      </c>
+      <c r="C52" s="4">
+        <v>1.1938618608046472</v>
       </c>
       <c r="D52" s="5">
-        <v>922</v>
+        <v>786</v>
       </c>
       <c r="E52" s="4">
-        <v>-4.4559585492227945E-2</v>
+        <v>1.0793650793650795</v>
       </c>
       <c r="F52" s="3">
-        <v>5.4400108459869845</v>
-      </c>
-      <c r="G52" s="6">
-        <v>5.1520404290008592E-2</v>
+        <v>5.3912340966921111</v>
+      </c>
+      <c r="G52" s="4">
+        <v>5.5063337638876053E-2</v>
       </c>
       <c r="H52" s="4">
-        <v>-7.0735361167198585E-2</v>
+        <v>0.41045880611741481</v>
       </c>
       <c r="I52" s="4">
-        <v>-0.16746529877625338</v>
+        <v>3.4961183276847052E-2</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
@@ -2125,28 +2125,28 @@
         <v>59</v>
       </c>
       <c r="B53" s="3">
-        <v>4992.4000000000015</v>
-      </c>
-      <c r="C53" s="6">
-        <v>0.22172001066961688</v>
+        <v>1931.5299999999997</v>
+      </c>
+      <c r="C53" s="4">
+        <v>2.7316678810958228E-2</v>
       </c>
       <c r="D53" s="5">
-        <v>965</v>
-      </c>
-      <c r="E53" s="6">
-        <v>0.18842364532019709</v>
+        <v>378</v>
+      </c>
+      <c r="E53" s="4">
+        <v>0.10850439882697938</v>
       </c>
       <c r="F53" s="3">
-        <v>5.173471502590675</v>
+        <v>5.1098677248677244</v>
       </c>
       <c r="G53" s="6">
-        <v>2.8017252501273404E-2</v>
+        <v>-7.3240773876886767E-2</v>
       </c>
       <c r="H53" s="6">
-        <v>0.29901006853371692</v>
+        <v>-3.171873507213141E-2</v>
       </c>
       <c r="I53" s="6">
-        <v>1.7412601716752629E-2</v>
+        <v>-8.6271938993084843E-2</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
@@ -2154,28 +2154,28 @@
         <v>60</v>
       </c>
       <c r="B54" s="3">
-        <v>4086.369999999999</v>
+        <v>1880.1700000000003</v>
       </c>
       <c r="C54" s="6">
-        <v>0.19001537619252809</v>
+        <v>-7.6523720879973389E-2</v>
       </c>
       <c r="D54" s="5">
-        <v>812</v>
+        <v>341</v>
       </c>
       <c r="E54" s="6">
-        <v>0.17171717171717168</v>
+        <v>-6.0606060606060552E-2</v>
       </c>
       <c r="F54" s="3">
-        <v>5.032475369458127</v>
+        <v>5.5136950146627575</v>
       </c>
       <c r="G54" s="6">
-        <v>1.5616571060864448E-2</v>
+        <v>-1.6944606098036163E-2</v>
       </c>
       <c r="H54" s="4">
-        <v>-2.0714226530781366E-2</v>
-      </c>
-      <c r="I54" s="4">
-        <v>-5.5765589854768309E-2</v>
+        <v>1.3164262898073709E-2</v>
+      </c>
+      <c r="I54" s="6">
+        <v>-6.6772432529096371E-2</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
@@ -2183,28 +2183,28 @@
         <v>61</v>
       </c>
       <c r="B55" s="3">
-        <v>3433.8800000000006</v>
-      </c>
-      <c r="C55" s="4">
-        <v>-0.29802196364468936</v>
+        <v>2035.9699999999998</v>
+      </c>
+      <c r="C55" s="6">
+        <v>-0.10456432630227151</v>
       </c>
       <c r="D55" s="5">
-        <v>693</v>
-      </c>
-      <c r="E55" s="4">
-        <v>-0.32718446601941747</v>
+        <v>363</v>
+      </c>
+      <c r="E55" s="6">
+        <v>-0.17123287671232881</v>
       </c>
       <c r="F55" s="3">
-        <v>4.9550937950937959</v>
-      </c>
-      <c r="G55" s="6">
-        <v>4.3343978998513721E-2</v>
-      </c>
-      <c r="H55" s="4">
-        <v>-9.3850889706434404E-2</v>
+        <v>5.6087327823691453</v>
+      </c>
+      <c r="G55" s="4">
+        <v>8.04430442964328E-2</v>
+      </c>
+      <c r="H55" s="6">
+        <v>-0.10939655172413797</v>
       </c>
       <c r="I55" s="4">
-        <v>-0.24332166327381288</v>
+        <v>0.30962342717725533</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -2212,28 +2212,28 @@
         <v>62</v>
       </c>
       <c r="B56" s="3">
-        <v>4891.72</v>
+        <v>2273.7200000000007</v>
       </c>
       <c r="C56" s="6">
-        <v>4.2792763985351145E-2</v>
+        <v>-0.29984880537772463</v>
       </c>
       <c r="D56" s="5">
-        <v>1030</v>
+        <v>438</v>
       </c>
       <c r="E56" s="6">
-        <v>0.17848970251716256</v>
+        <v>-0.22751322751322756</v>
       </c>
       <c r="F56" s="3">
-        <v>4.7492427184466024</v>
-      </c>
-      <c r="G56" s="4">
-        <v>-0.11514478085126513</v>
-      </c>
-      <c r="H56" s="4">
-        <v>-8.2081323225361769E-2</v>
+        <v>5.1911415525114171</v>
+      </c>
+      <c r="G56" s="6">
+        <v>-9.3639891893081972E-2</v>
+      </c>
+      <c r="H56" s="6">
+        <v>-4.5188904436579191E-2</v>
       </c>
       <c r="I56" s="6">
-        <v>0.25736888635241773</v>
+        <v>-3.3930588585017851E-2</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
@@ -2241,28 +2241,28 @@
         <v>63</v>
       </c>
       <c r="B57" s="3">
-        <v>4690.9799999999977</v>
+        <v>3247.4700000000003</v>
       </c>
       <c r="C57" s="6">
-        <v>4.2324186201532665E-2</v>
+        <v>-0.35253773658260379</v>
       </c>
       <c r="D57" s="5">
-        <v>874</v>
-      </c>
-      <c r="E57" s="4">
-        <v>-1.4656144306651631E-2</v>
+        <v>567</v>
+      </c>
+      <c r="E57" s="6">
+        <v>-0.38503253796095449</v>
       </c>
       <c r="F57" s="3">
-        <v>5.3672540045766564</v>
-      </c>
-      <c r="G57" s="6">
-        <v>5.7827864028328957E-2</v>
+        <v>5.7274603174603183</v>
+      </c>
+      <c r="G57" s="4">
+        <v>5.2839871024408014E-2</v>
       </c>
       <c r="H57" s="6">
-        <v>7.7528590524283292E-2</v>
+        <v>-0.14845447536272516</v>
       </c>
       <c r="I57" s="6">
-        <v>0.11618328947514132</v>
+        <v>-6.4403166181090321E-2</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
@@ -2270,28 +2270,28 @@
         <v>64</v>
       </c>
       <c r="B58" s="3">
-        <v>4500.5</v>
-      </c>
-      <c r="C58" s="6">
-        <v>1.8927301953859388E-2</v>
+        <v>5015.6900000000005</v>
+      </c>
+      <c r="C58" s="4">
+        <v>4.6650909382262018E-3</v>
       </c>
       <c r="D58" s="5">
-        <v>887</v>
-      </c>
-      <c r="E58" s="4">
-        <v>-2.9540481400437635E-2</v>
+        <v>922</v>
+      </c>
+      <c r="E58" s="6">
+        <v>-4.4559585492227945E-2</v>
       </c>
       <c r="F58" s="3">
-        <v>5.0738444193912065</v>
-      </c>
-      <c r="G58" s="6">
-        <v>4.9943127379737717E-2</v>
+        <v>5.4400108459869854</v>
+      </c>
+      <c r="G58" s="4">
+        <v>5.1520404290008814E-2</v>
       </c>
       <c r="H58" s="6">
-        <v>0.14351222826086962</v>
-      </c>
-      <c r="I58" s="4">
-        <v>-0.13087287630581856</v>
+        <v>-7.0735361167198585E-2</v>
+      </c>
+      <c r="I58" s="6">
+        <v>-0.16746529877625338</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
@@ -2299,28 +2299,28 @@
         <v>65</v>
       </c>
       <c r="B59" s="3">
-        <v>4416.8999999999987</v>
-      </c>
-      <c r="C59" s="6">
-        <v>0.17798135776293122</v>
+        <v>4992.4000000000005</v>
+      </c>
+      <c r="C59" s="4">
+        <v>0.22172001066961666</v>
       </c>
       <c r="D59" s="5">
-        <v>914</v>
-      </c>
-      <c r="E59" s="6">
-        <v>0.28913963328631875</v>
+        <v>965</v>
+      </c>
+      <c r="E59" s="4">
+        <v>0.18842364532019709</v>
       </c>
       <c r="F59" s="3">
-        <v>4.8324945295404804</v>
+        <v>5.1734715025906741</v>
       </c>
       <c r="G59" s="4">
-        <v>-8.6226714820658371E-2</v>
+        <v>2.8017252501273404E-2</v>
       </c>
       <c r="H59" s="4">
-        <v>-2.8623278066485236E-2</v>
+        <v>0.29901006853371692</v>
       </c>
       <c r="I59" s="4">
-        <v>-3.5689409053384691E-2</v>
+        <v>1.7412601716752629E-2</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
@@ -2328,28 +2328,28 @@
         <v>66</v>
       </c>
       <c r="B60" s="3">
-        <v>3749.55</v>
-      </c>
-      <c r="C60" s="6">
-        <v>1.4507984025412926</v>
+        <v>4086.369999999999</v>
+      </c>
+      <c r="C60" s="4">
+        <v>0.19001537619252828</v>
       </c>
       <c r="D60" s="5">
-        <v>709</v>
-      </c>
-      <c r="E60" s="6">
-        <v>1.6455223880597014</v>
+        <v>812</v>
+      </c>
+      <c r="E60" s="4">
+        <v>0.17171717171717168</v>
       </c>
       <c r="F60" s="3">
-        <v>5.2885049365303249</v>
+        <v>5.032475369458127</v>
       </c>
       <c r="G60" s="4">
-        <v>-7.3605117234038953E-2</v>
+        <v>1.561657106086467E-2</v>
       </c>
       <c r="H60" s="6">
-        <v>0.56850821581058342</v>
+        <v>-2.0714226530781366E-2</v>
       </c>
       <c r="I60" s="6">
-        <v>0.10364464767343229</v>
+        <v>-5.5765589854768309E-2</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
@@ -2357,28 +2357,28 @@
         <v>67</v>
       </c>
       <c r="B61" s="3">
-        <v>1529.9300000000005</v>
-      </c>
-      <c r="C61" s="4">
-        <v>-0.20620022310426245</v>
+        <v>3433.8799999999997</v>
+      </c>
+      <c r="C61" s="6">
+        <v>-0.29802196364468936</v>
       </c>
       <c r="D61" s="5">
-        <v>268</v>
-      </c>
-      <c r="E61" s="4">
-        <v>-0.1728395061728395</v>
+        <v>693</v>
+      </c>
+      <c r="E61" s="6">
+        <v>-0.32718446601941747</v>
       </c>
       <c r="F61" s="3">
-        <v>5.708694029850748</v>
+        <v>4.955093795093795</v>
       </c>
       <c r="G61" s="4">
-        <v>-4.0331613006645665E-2</v>
-      </c>
-      <c r="H61" s="4">
-        <v>-6.0532393339005723E-2</v>
+        <v>4.3343978998513721E-2</v>
+      </c>
+      <c r="H61" s="6">
+        <v>-9.3850889706434404E-2</v>
       </c>
       <c r="I61" s="6">
-        <v>0.38790959331779634</v>
+        <v>-0.24332166327381288</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
@@ -2386,28 +2386,28 @@
         <v>68</v>
       </c>
       <c r="B62" s="3">
-        <v>1927.3500000000008</v>
+        <v>4891.7199999999993</v>
       </c>
       <c r="C62" s="4">
-        <v>-0.1175096955572138</v>
+        <v>4.2792763985350923E-2</v>
       </c>
       <c r="D62" s="5">
-        <v>324</v>
+        <v>1030</v>
       </c>
       <c r="E62" s="4">
-        <v>-0.22857142857142854</v>
+        <v>0.17848970251716256</v>
       </c>
       <c r="F62" s="3">
-        <v>5.9486111111111137</v>
+        <v>4.7492427184466015</v>
       </c>
       <c r="G62" s="6">
-        <v>0.14396891316657467</v>
-      </c>
-      <c r="H62" s="4">
-        <v>-7.8826559175904198E-2</v>
+        <v>-0.11514478085126523</v>
+      </c>
+      <c r="H62" s="6">
+        <v>-8.2081323225361769E-2</v>
       </c>
       <c r="I62" s="4">
-        <v>-0.20843715813783881</v>
+        <v>0.25736888635241773</v>
       </c>
     </row>
   </sheetData>

</xml_diff>